<commit_message>
Fix enrollment upload: PSL time filtering, preview format, and step navigation
</commit_message>
<xml_diff>
--- a/assets/Blank_MTWT_Template1.xlsx
+++ b/assets/Blank_MTWT_Template1.xlsx
@@ -539,7 +539,11 @@
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Liam (3); Neil (8)</t>
+        </is>
+      </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
@@ -563,7 +567,11 @@
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Paul (3); Tara (7)</t>
+        </is>
+      </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
@@ -587,7 +595,11 @@
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Anqi (32); Riyansh (10)</t>
+        </is>
+      </c>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
@@ -611,7 +623,11 @@
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Varun (13); Amyra (6)</t>
+        </is>
+      </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
@@ -635,7 +651,11 @@
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Hugh (7); Myra (9)</t>
+        </is>
+      </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
@@ -659,7 +679,11 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Hugh (7)</t>
+        </is>
+      </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>

</xml_diff>

<commit_message>
Fix enrollment parsing: day of week filtering, date range logic, and step 2 navigation
</commit_message>
<xml_diff>
--- a/assets/Blank_MTWT_Template1.xlsx
+++ b/assets/Blank_MTWT_Template1.xlsx
@@ -539,11 +539,7 @@
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Liam (3); Neil (8)</t>
-        </is>
-      </c>
+      <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
@@ -567,11 +563,7 @@
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Paul (3); Tara (7)</t>
-        </is>
-      </c>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
@@ -595,11 +587,7 @@
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Anqi (32); Riyansh (10)</t>
-        </is>
-      </c>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
@@ -623,11 +611,7 @@
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Varun (13); Amyra (6)</t>
-        </is>
-      </c>
+      <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
@@ -651,11 +635,7 @@
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Hugh (7); Myra (9)</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
@@ -679,11 +659,7 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Hugh (7)</t>
-        </is>
-      </c>
+      <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>

</xml_diff>

<commit_message>
V2.4- Instructor accounts and database added!! More features coming tonight# Please enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/assets/Blank_MTWT_Template1.xlsx
+++ b/assets/Blank_MTWT_Template1.xlsx
@@ -529,7 +529,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>4:10</t>
+          <t>8:35</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -553,7 +553,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>4:45</t>
+          <t>9:10</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -577,7 +577,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>5:20</t>
+          <t>9:45</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -601,7 +601,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>5:55</t>
+          <t>10:20</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -625,7 +625,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>6:30</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -649,7 +649,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>7:05</t>
+          <t>11:35</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>

</xml_diff>